<commit_message>
slmatches through summer 21
</commit_message>
<xml_diff>
--- a/data/slmatchups/SLMatchupAverages.xlsx
+++ b/data/slmatchups/SLMatchupAverages.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24931"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/d53cb9c05b082722/Documents/apa-rankings/data/slmatchups/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="2" documentId="11_6A69D6BF8740DDF6313BF892443088B35299F7C6" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{202AA3CC-8144-4A47-ABE4-9150A2191829}"/>
+  <xr:revisionPtr revIDLastSave="1" documentId="11_6A69D6BF87B0512BE5CC5611413088B35299F7BD" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D6E57ADC-E292-4D7B-9F1C-628E175C6D35}"/>
   <bookViews>
     <workbookView xWindow="21300" yWindow="1440" windowWidth="15150" windowHeight="11025" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,18 +20,9 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1" uniqueCount="1">
   <si>
     <t>SL</t>
-  </si>
-  <si>
-    <t>X0.0</t>
-  </si>
-  <si>
-    <t>X2.0</t>
-  </si>
-  <si>
-    <t>X3.0</t>
   </si>
 </sst>
 </file>
@@ -92,9 +83,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -400,7 +389,7 @@
   <dimension ref="A1:G7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J16" sqref="J16"/>
+      <selection activeCell="J11" sqref="J11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -436,16 +425,16 @@
         <v>1.5</v>
       </c>
       <c r="C2" s="2">
-        <v>1.59</v>
+        <v>1.4</v>
       </c>
       <c r="D2" s="2">
-        <v>1.43</v>
-      </c>
-      <c r="E2" s="2" t="s">
+        <v>1.19</v>
+      </c>
+      <c r="E2" s="2">
         <v>1</v>
       </c>
-      <c r="F2" s="2" t="s">
-        <v>2</v>
+      <c r="F2" s="2">
+        <v>1.33</v>
       </c>
       <c r="G2" s="2">
         <v>0.5</v>
@@ -456,7 +445,7 @@
         <v>3</v>
       </c>
       <c r="B3" s="2">
-        <v>1.26</v>
+        <v>1.4</v>
       </c>
       <c r="C3" s="2">
         <v>1.5</v>
@@ -465,10 +454,10 @@
         <v>1.4</v>
       </c>
       <c r="E3" s="2">
-        <v>1.64</v>
+        <v>1.37</v>
       </c>
       <c r="F3" s="2">
-        <v>1.29</v>
+        <v>1</v>
       </c>
       <c r="G3" s="2">
         <v>1</v>
@@ -479,68 +468,68 @@
         <v>4</v>
       </c>
       <c r="B4" s="2">
-        <v>1.43</v>
+        <v>1.56</v>
       </c>
       <c r="C4" s="2">
-        <v>1.37</v>
+        <v>1.44</v>
       </c>
       <c r="D4" s="2">
-        <v>1.35</v>
+        <v>1.38</v>
       </c>
       <c r="E4" s="2">
-        <v>1.22</v>
+        <v>1.24</v>
       </c>
       <c r="F4" s="2">
-        <v>1.25</v>
+        <v>1.1200000000000001</v>
       </c>
       <c r="G4" s="2">
-        <v>0</v>
+        <v>0.56999999999999995</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>5</v>
       </c>
-      <c r="B5" s="2" t="s">
-        <v>3</v>
+      <c r="B5" s="2">
+        <v>2</v>
       </c>
       <c r="C5" s="2">
-        <v>1</v>
+        <v>1.33</v>
       </c>
       <c r="D5" s="2">
-        <v>1.33</v>
+        <v>1.35</v>
       </c>
       <c r="E5" s="2">
         <v>1.22</v>
       </c>
       <c r="F5" s="2">
-        <v>1.1599999999999999</v>
+        <v>1.17</v>
       </c>
       <c r="G5" s="2">
-        <v>0.14000000000000001</v>
+        <v>0.72</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>6</v>
       </c>
-      <c r="B6" s="2" t="s">
+      <c r="B6" s="2">
         <v>1</v>
       </c>
       <c r="C6" s="2">
-        <v>1.1399999999999999</v>
+        <v>1.64</v>
       </c>
       <c r="D6" s="2">
-        <v>1.42</v>
+        <v>1.56</v>
       </c>
       <c r="E6" s="2">
-        <v>1.22</v>
+        <v>1.21</v>
       </c>
       <c r="F6" s="2">
-        <v>1.08</v>
+        <v>1.0900000000000001</v>
       </c>
       <c r="G6" s="2">
-        <v>1.22</v>
+        <v>1.1299999999999999</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
@@ -551,19 +540,19 @@
         <v>2.5</v>
       </c>
       <c r="C7" s="2">
-        <v>1.75</v>
+        <v>1.8</v>
       </c>
       <c r="D7" s="2">
-        <v>3</v>
+        <v>2.29</v>
       </c>
       <c r="E7" s="2">
-        <v>2.71</v>
+        <v>1.89</v>
       </c>
       <c r="F7" s="2">
-        <v>1.39</v>
+        <v>1.43</v>
       </c>
       <c r="G7" s="2">
-        <v>1.25</v>
+        <v>1.2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>